<commit_message>
Updated spelling and removed stress soon be raplaced with area
</commit_message>
<xml_diff>
--- a/spalling.xlsx
+++ b/spalling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delto\Dropbox\python\Concrete\Spalling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD573D39-8254-42BC-A0DE-E5054A95896B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC134E1-DAFB-4564-BA42-785C95126208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{626C1325-BBAB-40E7-B20C-582232EBEF2A}"/>
+    <workbookView xWindow="-20617" yWindow="-3517" windowWidth="20715" windowHeight="13425" xr2:uid="{626C1325-BBAB-40E7-B20C-582232EBEF2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E074AA0D-D2A1-4FF3-982D-53F03511EBB6}">
   <dimension ref="A1:J175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>